<commit_message>
fixed : validity date with quarter notation
</commit_message>
<xml_diff>
--- a/public/data/db_source/variable.xlsx
+++ b/public/data/db_source/variable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E73312-261D-B341-B7EB-71BD0C0FA7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA23BEE-C9E6-314E-B935-5859479D7D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3680" windowWidth="28800" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2516" uniqueCount="1287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2516" uniqueCount="1291">
   <si>
     <t>id</t>
   </si>
@@ -3881,6 +3881,18 @@
   </si>
   <si>
     <t>description of variable 36</t>
+  </si>
+  <si>
+    <t>2021/02</t>
+  </si>
+  <si>
+    <t>2020t2</t>
+  </si>
+  <si>
+    <t>2020t3</t>
+  </si>
+  <si>
+    <t>2018t4</t>
   </si>
 </sst>
 </file>
@@ -4260,11 +4272,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M603"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I47" sqref="I47"/>
+      <selection pane="bottomRight" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5089,7 +5101,7 @@
         <v>1271</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>85</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -5115,7 +5127,7 @@
         <v>94</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>99</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -5167,7 +5179,7 @@
         <v>94</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>99</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -5207,7 +5219,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>94</v>
+        <v>1290</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
fixed : jsonjsdb_editor - history file was not included if no change
</commit_message>
<xml_diff>
--- a/public/data/db_source/variable.xlsx
+++ b/public/data/db_source/variable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA23BEE-C9E6-314E-B935-5859479D7D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64BA5EC-D37D-F94E-9465-C77DA590C4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3680" windowWidth="28800" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4276,7 +4276,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J49" sqref="J49"/>
+      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5193,7 +5193,7 @@
         <v>97</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I45" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
changed : make jsonjsdb_editor use xlsx state for evolution
</commit_message>
<xml_diff>
--- a/public/data/db_source/variable.xlsx
+++ b/public/data/db_source/variable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64BA5EC-D37D-F94E-9465-C77DA590C4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3B8826-2625-6247-A1EA-CCC0BACA51E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3680" windowWidth="28800" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5236,7 +5236,7 @@
         <v>100</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I47" t="s">
         <v>40</v>

</xml_diff>